<commit_message>
update output data prep
</commit_message>
<xml_diff>
--- a/spine_projects/02_output_data/01_basic_energy_model_outputs/output_last_run.xlsx
+++ b/spine_projects/02_output_data/01_basic_energy_model_outputs/output_last_run.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM27"/>
+  <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,15 +611,35 @@
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
+          <t>unit_flow.17</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>unit_flow.18</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>unit_flow.19</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>unit_flow.20</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
           <t>unit_flow_op</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>proceeds from PV</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>adjusted costs</t>
         </is>
@@ -806,11 +826,31 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
+          <t>Steam_Plant</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>Steam_Plant</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>Steam_Plant</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>Steam_Plant</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
           <t>Electrolyzer</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -980,8 +1020,28 @@
           <t>from_node</t>
         </is>
       </c>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1159,8 +1219,28 @@
           <t>Power_Kasso</t>
         </is>
       </c>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>Steam</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1172,10 +1252,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1205,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>21.87434817803732</v>
+        <v>43.84938177476902</v>
       </c>
       <c r="O5" t="n">
-        <v>21.87434817803732</v>
+        <v>43.84938177476902</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -1220,19 +1300,19 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-94996.28761344512</v>
+        <v>-94427.62279218005</v>
       </c>
       <c r="T5" t="n">
         <v>7.167792870282449</v>
       </c>
       <c r="U5" t="n">
-        <v>0.02555362877106043</v>
+        <v>0.02555362877106042</v>
       </c>
       <c r="V5" t="n">
         <v>7.167792870282449</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>0.04807692307692308</v>
       </c>
       <c r="X5" t="n">
         <v>31.44654088050315</v>
@@ -1244,13 +1324,13 @@
         <v>25</v>
       </c>
       <c r="AA5" t="n">
-        <v>21.84879454926626</v>
+        <v>43.67575122292104</v>
       </c>
       <c r="AB5" t="n">
-        <v>3468.06262686766</v>
+        <v>7465.940379986502</v>
       </c>
       <c r="AC5" t="n">
-        <v>32.75681341719079</v>
+        <v>32.75681341719078</v>
       </c>
       <c r="AD5" t="n">
         <v>18.61182580522204</v>
@@ -1259,7 +1339,7 @@
         <v>32.75681341719079</v>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG5" t="n">
         <v>7.167792870282448</v>
@@ -1273,12 +1353,24 @@
       <c r="AJ5" t="n">
         <v>0</v>
       </c>
-      <c r="AK5" t="inlineStr"/>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
       <c r="AL5" t="n">
+        <v>25.89111767570888</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>5.178223535141776</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>2.622730682277159</v>
+      </c>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="n">
         <v>-0</v>
       </c>
-      <c r="AM5" t="n">
-        <v>-92232.70873344512</v>
+      <c r="AQ5" t="n">
+        <v>-94427.62279218005</v>
       </c>
     </row>
     <row r="6">
@@ -1291,13 +1383,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>4.330000000000004</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1306,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>4.330000000000004</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1324,77 +1416,89 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>21.87434817803732</v>
+        <v>7.67739292339</v>
       </c>
       <c r="O6" t="n">
-        <v>21.87434817803732</v>
+        <v>7.67739292339</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>4.330000000000004</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
-        <v>7.167792870282449</v>
+        <v>1.241461725132921</v>
       </c>
       <c r="U6" t="n">
-        <v>0.02555362877106043</v>
+        <v>0.004425888503147669</v>
       </c>
       <c r="V6" t="n">
-        <v>7.167792870282449</v>
+        <v>1.241461725132921</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>0.008326923076923084</v>
       </c>
       <c r="X6" t="n">
-        <v>31.44654088050315</v>
+        <v>5.44654088050315</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.62273068227716</v>
+        <v>0.4542569541704045</v>
       </c>
       <c r="Z6" t="n">
-        <v>25</v>
+        <v>4.330000000000004</v>
       </c>
       <c r="AA6" t="n">
-        <v>21.84879454926626</v>
+        <v>7.56464011180993</v>
       </c>
       <c r="AB6" t="n">
-        <v>3468.06262686766</v>
+        <v>1293.100873813663</v>
       </c>
       <c r="AC6" t="n">
-        <v>32.75681341719079</v>
+        <v>5.673480083857449</v>
       </c>
       <c r="AD6" t="n">
-        <v>18.61182580522204</v>
+        <v>3.22356822946446</v>
       </c>
       <c r="AE6" t="n">
-        <v>32.75681341719079</v>
+        <v>5.67348008385745</v>
       </c>
       <c r="AF6" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG6" t="n">
-        <v>7.167792870282448</v>
+        <v>1.241461725132921</v>
       </c>
       <c r="AH6" t="n">
-        <v>31.44654088050315</v>
+        <v>5.44654088050315</v>
       </c>
       <c r="AI6" t="n">
-        <v>7.27929187048684</v>
+        <v>1.260773351968322</v>
       </c>
       <c r="AJ6" t="n">
         <v>0</v>
       </c>
-      <c r="AK6" t="inlineStr"/>
+      <c r="AK6" t="n">
+        <v>0</v>
+      </c>
       <c r="AL6" t="n">
+        <v>4.484341581432782</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.8968683162865564</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.4542569541704045</v>
+      </c>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="n">
         <v>-0</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1406,25 +1510,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>40.35907423289502</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>40.35907423289502</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>13.97000000000001</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>4.330000000000005</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>4.330000000000005</v>
       </c>
       <c r="H7" t="n">
-        <v>13.97000000000001</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>11.91666666666667</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -1433,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>11.91666666666667</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1448,68 +1552,80 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>13.97000000000001</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>11.91666666666667</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
-        <v>11.17315552619628</v>
+        <v>5.926331145149526</v>
       </c>
       <c r="U7" t="n">
-        <v>0.039832996528329</v>
+        <v>0.02112774026791275</v>
       </c>
       <c r="V7" t="n">
-        <v>11.17315552619628</v>
+        <v>5.926331145149526</v>
       </c>
       <c r="W7" t="n">
-        <v>965.9022660600755</v>
+        <v>0.03974999999999999</v>
       </c>
       <c r="X7" t="n">
-        <v>49.01886792452832</v>
+        <v>26</v>
       </c>
       <c r="Y7" t="n">
-        <v>4.088312587533638</v>
+        <v>2.168473728106755</v>
       </c>
       <c r="Z7" t="n">
-        <v>38.97000000000001</v>
+        <v>20.66999999999999</v>
       </c>
       <c r="AA7" t="n">
-        <v>34.05790094339626</v>
+        <v>51.99999999999999</v>
       </c>
       <c r="AB7" t="n">
-        <v>5406.016022761311</v>
+        <v>8888.888888888887</v>
       </c>
       <c r="AC7" t="n">
-        <v>51.06132075471703</v>
+        <v>39</v>
       </c>
       <c r="AD7" t="n">
-        <v>29.01211406518013</v>
+        <v>22.15909090909091</v>
       </c>
       <c r="AE7" t="n">
-        <v>51.06132075471702</v>
+        <v>27.08333333333334</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG7" t="n">
-        <v>11.17315552619628</v>
+        <v>5.926331145149526</v>
       </c>
       <c r="AH7" t="n">
-        <v>49.01886792452832</v>
+        <v>26</v>
       </c>
       <c r="AI7" t="n">
-        <v>11.34696016771489</v>
+        <v>6.018518518518517</v>
       </c>
       <c r="AJ7" t="n">
         <v>0</v>
       </c>
-      <c r="AK7" t="inlineStr"/>
+      <c r="AK7" t="n">
+        <v>947.839122259732</v>
+      </c>
       <c r="AL7" t="n">
+        <v>28.17760942760943</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>5.635521885521886</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>2.168473728106755</v>
+      </c>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="n">
         <v>-0</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1521,13 +1637,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40.35907423289502</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>40.35907423289502</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>13.97000000000001</v>
+        <v>28.85959999999996</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1536,16 +1652,16 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>13.97000000000001</v>
+        <v>28.85959999999996</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>11.91666666666667</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>11.91666666666667</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -1563,68 +1679,80 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>27.94000000000002</v>
+        <v>28.85959999999996</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
-        <v>11.17315552619628</v>
+        <v>11.1415025528811</v>
       </c>
       <c r="U8" t="n">
-        <v>0.039832996528329</v>
+        <v>0.03972015170367595</v>
       </c>
       <c r="V8" t="n">
-        <v>11.17315552619628</v>
+        <v>11.1415025528811</v>
       </c>
       <c r="W8" t="n">
-        <v>965.9022660600755</v>
+        <v>0.07472999999999994</v>
       </c>
       <c r="X8" t="n">
-        <v>49.01886792452832</v>
+        <v>48.87999999999996</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.088312587533638</v>
+        <v>4.076730608840697</v>
       </c>
       <c r="Z8" t="n">
-        <v>38.97000000000001</v>
+        <v>38.85959999999996</v>
       </c>
       <c r="AA8" t="n">
-        <v>34.05790094339626</v>
+        <v>51.99999999999994</v>
       </c>
       <c r="AB8" t="n">
-        <v>5406.016022761311</v>
+        <v>8888.888888888878</v>
       </c>
       <c r="AC8" t="n">
-        <v>51.06132075471703</v>
+        <v>38.99999999999996</v>
       </c>
       <c r="AD8" t="n">
-        <v>29.01211406518013</v>
+        <v>22.15909090909089</v>
       </c>
       <c r="AE8" t="n">
-        <v>51.06132075471702</v>
+        <v>50.91666666666664</v>
       </c>
       <c r="AF8" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG8" t="n">
-        <v>11.17315552619628</v>
+        <v>11.1415025528811</v>
       </c>
       <c r="AH8" t="n">
-        <v>49.01886792452832</v>
+        <v>48.87999999999996</v>
       </c>
       <c r="AI8" t="n">
-        <v>11.34696016771489</v>
+        <v>11.3148148148148</v>
       </c>
       <c r="AJ8" t="n">
         <v>0</v>
       </c>
-      <c r="AK8" t="inlineStr"/>
+      <c r="AK8" t="n">
+        <v>947.7855498482963</v>
+      </c>
       <c r="AL8" t="n">
+        <v>33.47390572390569</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>6.694781144781139</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>4.076730608840696</v>
+      </c>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="n">
         <v>-0</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1636,25 +1764,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>16.34</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>2.235200000000006</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>2.235200000000006</v>
       </c>
       <c r="H9" t="n">
-        <v>16.34</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5.329070518200754e-15</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1663,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>5.329070518200754e-15</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -1678,68 +1806,80 @@
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>44.28000000000002</v>
+        <v>26.62439999999996</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="n">
-        <v>11.85266229029905</v>
+        <v>8.53391684901532</v>
       </c>
       <c r="U9" t="n">
-        <v>0.04225548053582551</v>
+        <v>0.03042394598579437</v>
       </c>
       <c r="V9" t="n">
-        <v>11.85266229029905</v>
+        <v>8.53391684901532</v>
       </c>
       <c r="W9" t="n">
-        <v>963.8285778527976</v>
+        <v>0.05723999999999999</v>
       </c>
       <c r="X9" t="n">
+        <v>37.44</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>29.76479999999999</v>
+      </c>
+      <c r="AA9" t="n">
         <v>52</v>
       </c>
-      <c r="Y9" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>36.12916666666668</v>
-      </c>
       <c r="AB9" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC9" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD9" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE9" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AF9" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG9" t="n">
-        <v>11.85266229029905</v>
+        <v>8.533916849015318</v>
       </c>
       <c r="AH9" t="n">
-        <v>52</v>
+        <v>37.44</v>
       </c>
       <c r="AI9" t="n">
-        <v>12.03703703703704</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="AJ9" t="n">
         <v>0</v>
       </c>
-      <c r="AK9" t="inlineStr"/>
+      <c r="AK9" t="n">
+        <v>947.8123360540142</v>
+      </c>
       <c r="AL9" t="n">
+        <v>30.82575757575758</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>6.165151515151517</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="n">
         <v>-0</v>
       </c>
-      <c r="AM9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1751,13 +1891,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>16.34</v>
+        <v>9.764799999999994</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1766,10 +1906,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>16.34</v>
+        <v>9.764799999999994</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>5.329070518200754e-15</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -1778,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>5.329070518200754e-15</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1793,68 +1933,80 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>60.62000000000001</v>
+        <v>36.38919999999995</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="n">
-        <v>11.85266229029905</v>
+        <v>8.53391684901532</v>
       </c>
       <c r="U10" t="n">
-        <v>0.04225548053582551</v>
+        <v>0.03042394598579437</v>
       </c>
       <c r="V10" t="n">
-        <v>11.85266229029905</v>
+        <v>8.53391684901532</v>
       </c>
       <c r="W10" t="n">
-        <v>963.8285778527976</v>
+        <v>0.05723999999999999</v>
       </c>
       <c r="X10" t="n">
+        <v>37.44</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>29.76479999999999</v>
+      </c>
+      <c r="AA10" t="n">
         <v>52</v>
       </c>
-      <c r="Y10" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>36.12916666666668</v>
-      </c>
       <c r="AB10" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC10" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD10" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE10" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AF10" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG10" t="n">
-        <v>11.85266229029905</v>
+        <v>8.533916849015318</v>
       </c>
       <c r="AH10" t="n">
-        <v>52</v>
+        <v>37.44</v>
       </c>
       <c r="AI10" t="n">
-        <v>12.03703703703704</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="AJ10" t="n">
         <v>0</v>
       </c>
-      <c r="AK10" t="inlineStr"/>
+      <c r="AK10" t="n">
+        <v>947.8123360540142</v>
+      </c>
       <c r="AL10" t="n">
+        <v>30.82575757575758</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>6.165151515151517</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="n">
         <v>-0</v>
       </c>
-      <c r="AM10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1866,25 +2018,25 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>16.34</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1.983599999999274</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1.983599999999274</v>
       </c>
       <c r="H11" t="n">
-        <v>16.34</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>14.08333333333239</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -1893,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>14.08333333333239</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -1908,68 +2060,80 @@
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>76.96000000000001</v>
+        <v>34.40560000000067</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>14.08333333333465</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537774</v>
       </c>
       <c r="U11" t="n">
-        <v>0.04225548053582551</v>
+        <v>0.01943752104648048</v>
       </c>
       <c r="V11" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537774</v>
       </c>
       <c r="W11" t="n">
-        <v>963.8285778527976</v>
+        <v>0.0365700000000014</v>
       </c>
       <c r="X11" t="n">
+        <v>23.92000000000091</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>1.994995829858291</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>19.01640000000073</v>
+      </c>
+      <c r="AA11" t="n">
         <v>52</v>
       </c>
-      <c r="Y11" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>36.12916666666668</v>
-      </c>
       <c r="AB11" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC11" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD11" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE11" t="n">
-        <v>54.16666666666669</v>
+        <v>24.91666666666763</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG11" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537773</v>
       </c>
       <c r="AH11" t="n">
-        <v>52</v>
+        <v>23.92000000000091</v>
       </c>
       <c r="AI11" t="n">
-        <v>12.03703703703704</v>
+        <v>5.537037037037249</v>
       </c>
       <c r="AJ11" t="n">
         <v>0</v>
       </c>
-      <c r="AK11" t="inlineStr"/>
+      <c r="AK11" t="n">
+        <v>947.8439924789535</v>
+      </c>
       <c r="AL11" t="n">
+        <v>27.69612794612816</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>5.539225589225634</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>1.994995829858291</v>
+      </c>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="n">
         <v>-0</v>
       </c>
-      <c r="AM11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1981,13 +2145,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>16.34</v>
+        <v>4.016400000000608</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1996,10 +2160,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>16.34</v>
+        <v>4.016400000000608</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>14.08333333333254</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -2008,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>14.08333333333254</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -2023,68 +2187,80 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>93.30000000000001</v>
+        <v>38.42200000000128</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>28.16666666666718</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537741</v>
       </c>
       <c r="U12" t="n">
-        <v>0.04225548053582551</v>
+        <v>0.01943752104648036</v>
       </c>
       <c r="V12" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537741</v>
       </c>
       <c r="W12" t="n">
-        <v>963.8285778527976</v>
+        <v>0.03657000000000117</v>
       </c>
       <c r="X12" t="n">
+        <v>23.92000000000077</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>1.994995829858279</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>19.01640000000061</v>
+      </c>
+      <c r="AA12" t="n">
         <v>52</v>
       </c>
-      <c r="Y12" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>36.12916666666668</v>
-      </c>
       <c r="AB12" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC12" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD12" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE12" t="n">
-        <v>54.16666666666669</v>
+        <v>24.91666666666747</v>
       </c>
       <c r="AF12" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG12" t="n">
-        <v>11.85266229029905</v>
+        <v>5.452224653537741</v>
       </c>
       <c r="AH12" t="n">
-        <v>52</v>
+        <v>23.92000000000077</v>
       </c>
       <c r="AI12" t="n">
-        <v>12.03703703703704</v>
+        <v>5.537037037037215</v>
       </c>
       <c r="AJ12" t="n">
         <v>0</v>
       </c>
-      <c r="AK12" t="inlineStr"/>
+      <c r="AK12" t="n">
+        <v>947.8439924789535</v>
+      </c>
       <c r="AL12" t="n">
+        <v>27.69612794612813</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>5.539225589225627</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>1.994995829858279</v>
+      </c>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="n">
         <v>-0</v>
       </c>
-      <c r="AM12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -2096,13 +2272,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>16.34</v>
+        <v>34.68640000000037</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2111,16 +2287,16 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>16.34</v>
+        <v>34.68640000000037</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>13.00000000000049</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>13.00000000000049</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -2138,68 +2314,80 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>109.64</v>
+        <v>73.10840000000165</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>15.16666666666668</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
-        <v>11.85266229029905</v>
+        <v>11.3785557986872</v>
       </c>
       <c r="U13" t="n">
-        <v>0.04225548053582551</v>
+        <v>0.04056526131439287</v>
       </c>
       <c r="V13" t="n">
-        <v>11.85266229029905</v>
+        <v>11.3785557986872</v>
       </c>
       <c r="W13" t="n">
-        <v>963.8285778527976</v>
+        <v>0.07632000000000072</v>
       </c>
       <c r="X13" t="n">
+        <v>49.92000000000047</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>4.16346955796501</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>39.68640000000037</v>
+      </c>
+      <c r="AA13" t="n">
         <v>52</v>
       </c>
-      <c r="Y13" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>36.12916666666668</v>
-      </c>
       <c r="AB13" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC13" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD13" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE13" t="n">
-        <v>54.16666666666669</v>
+        <v>52.0000000000005</v>
       </c>
       <c r="AF13" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG13" t="n">
-        <v>11.85266229029905</v>
+        <v>11.3785557986872</v>
       </c>
       <c r="AH13" t="n">
-        <v>52</v>
+        <v>49.92000000000047</v>
       </c>
       <c r="AI13" t="n">
-        <v>12.03703703703704</v>
+        <v>11.55555555555566</v>
       </c>
       <c r="AJ13" t="n">
         <v>0</v>
       </c>
-      <c r="AK13" t="inlineStr"/>
+      <c r="AK13" t="n">
+        <v>947.7831147386855</v>
+      </c>
       <c r="AL13" t="n">
+        <v>33.71464646464658</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>6.742929292929316</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>4.163469557965009</v>
+      </c>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="n">
         <v>-0</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -2211,13 +2399,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>56.33307083831821</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>56.33307083831821</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>16.34</v>
+        <v>41.34</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2226,19 +2414,19 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>16.34</v>
+        <v>41.34</v>
       </c>
       <c r="I14" t="n">
-        <v>23.79435282358817</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="L14" t="n">
-        <v>23.79435282358817</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -2253,10 +2441,10 @@
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>125.98</v>
+        <v>114.4484000000016</v>
       </c>
       <c r="R14" t="n">
-        <v>23.79435282358817</v>
+        <v>0</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="n">
@@ -2269,7 +2457,7 @@
         <v>11.85266229029905</v>
       </c>
       <c r="W14" t="n">
-        <v>953.1257445194642</v>
+        <v>0.0795</v>
       </c>
       <c r="X14" t="n">
         <v>52</v>
@@ -2281,22 +2469,22 @@
         <v>41.34</v>
       </c>
       <c r="AA14" t="n">
-        <v>51.99999999999999</v>
+        <v>52.00000000000001</v>
       </c>
       <c r="AB14" t="n">
-        <v>8253.968253968253</v>
+        <v>8888.888888888891</v>
       </c>
       <c r="AC14" t="n">
-        <v>77.96101949025486</v>
+        <v>39.00000000000002</v>
       </c>
       <c r="AD14" t="n">
-        <v>44.29603380128117</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE14" t="n">
         <v>54.16666666666669</v>
       </c>
       <c r="AF14" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG14" t="n">
         <v>11.85266229029905</v>
@@ -2310,11 +2498,23 @@
       <c r="AJ14" t="n">
         <v>5.168</v>
       </c>
-      <c r="AK14" t="inlineStr"/>
+      <c r="AK14" t="n">
+        <v>952.9462445194641</v>
+      </c>
       <c r="AL14" t="n">
+        <v>34.19612794612796</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>6.839225589225592</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>4.336947456213511</v>
+      </c>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="n">
         <v>-0</v>
       </c>
-      <c r="AM14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2326,34 +2526,34 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7.887257444510095</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>7.887257444510095</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>16.31533333333484</v>
       </c>
       <c r="F15" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>16.31533333333484</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>4.519741439550783</v>
       </c>
       <c r="J15" t="n">
-        <v>23.79435282358817</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>23.79435282358817</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>4.519741439550783</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
@@ -2368,68 +2568,80 @@
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>121.65</v>
+        <v>130.7637333333365</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>4.519741439550772</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="n">
-        <v>5.926331145149527</v>
+        <v>7.544914345831342</v>
       </c>
       <c r="U15" t="n">
-        <v>0.02112774026791275</v>
+        <v>0.02689809035947002</v>
       </c>
       <c r="V15" t="n">
-        <v>5.926331145149527</v>
+        <v>7.544914345831342</v>
       </c>
       <c r="W15" t="n">
-        <v>1028.793122259732</v>
+        <v>0.05060641025641316</v>
       </c>
       <c r="X15" t="n">
-        <v>26</v>
+        <v>33.10104821803125</v>
       </c>
       <c r="Y15" t="n">
-        <v>2.168473728106755</v>
+        <v>2.760721285907527</v>
       </c>
       <c r="Z15" t="n">
-        <v>20.67</v>
+        <v>26.31533333333484</v>
       </c>
       <c r="AA15" t="n">
-        <v>2.193750000000033</v>
+        <v>52</v>
       </c>
       <c r="AB15" t="n">
-        <v>348.2142857142909</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC15" t="n">
-        <v>3.288980509745176</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD15" t="n">
-        <v>1.868738925991577</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE15" t="n">
-        <v>27.08333333333334</v>
+        <v>34.48025856044923</v>
       </c>
       <c r="AF15" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG15" t="n">
-        <v>5.926331145149527</v>
+        <v>7.544914345831341</v>
       </c>
       <c r="AH15" t="n">
-        <v>26</v>
+        <v>33.10104821803125</v>
       </c>
       <c r="AI15" t="n">
-        <v>6.018518518518518</v>
+        <v>7.662279680099826</v>
       </c>
       <c r="AJ15" t="n">
         <v>31.008</v>
       </c>
-      <c r="AK15" t="inlineStr"/>
+      <c r="AK15" t="n">
+        <v>978.8304954993843</v>
+      </c>
       <c r="AL15" t="n">
+        <v>29.82137058919074</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>5.964274117838149</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>2.760721285907527</v>
+      </c>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="n">
         <v>-0</v>
       </c>
-      <c r="AM15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2450,16 +2662,16 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>25</v>
+        <v>19.35466666666515</v>
       </c>
       <c r="G16" t="n">
-        <v>25</v>
+        <v>19.35466666666515</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>31.60307477288411</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -2468,83 +2680,95 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>31.60307477288411</v>
       </c>
       <c r="M16" t="n">
-        <v>51.072</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>1.044626760347962</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1.044626760347962</v>
       </c>
       <c r="P16" t="n">
-        <v>51.072</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>96.65000000000002</v>
+        <v>111.4090666666713</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>36.12281621243488</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>1.618583200681815</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
+        <v>0.005770350091557274</v>
       </c>
       <c r="V16" t="n">
-        <v>0</v>
+        <v>1.618583200681815</v>
       </c>
       <c r="W16" t="n">
-        <v>0</v>
+        <v>0.01085641025641317</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>7.101048218031259</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>0.5922475578007722</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>5.64533333333485</v>
       </c>
       <c r="AA16" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC16" t="n">
-        <v>0</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD16" t="n">
-        <v>0</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE16" t="n">
-        <v>0</v>
+        <v>7.396925227115897</v>
       </c>
       <c r="AF16" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG16" t="n">
-        <v>0</v>
+        <v>1.618583200681815</v>
       </c>
       <c r="AH16" t="n">
-        <v>0</v>
+        <v>7.101048218031259</v>
       </c>
       <c r="AI16" t="n">
-        <v>0</v>
+        <v>1.64376116158131</v>
       </c>
       <c r="AJ16" t="n">
         <v>51.072</v>
       </c>
-      <c r="AK16" t="inlineStr"/>
+      <c r="AK16" t="n">
+        <v>0</v>
+      </c>
       <c r="AL16" t="n">
-        <v>-1446.35904</v>
-      </c>
-      <c r="AM16" t="inlineStr"/>
+        <v>23.80285207067223</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>4.760570414134445</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>0.5922475578007722</v>
+      </c>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2562,19 +2786,19 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1.315333333334856</v>
       </c>
       <c r="F17" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1.315333333334856</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>4.519741439550767</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -2583,83 +2807,95 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>4.519741439550767</v>
       </c>
       <c r="M17" t="n">
-        <v>46.512</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>5.665504500615884</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>5.665504500615884</v>
       </c>
       <c r="P17" t="n">
-        <v>46.512</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>71.65000000000002</v>
+        <v>112.7244000000062</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>40.64255765198565</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>7.544914345831344</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
+        <v>0.02689809035947004</v>
       </c>
       <c r="V17" t="n">
-        <v>0</v>
+        <v>7.544914345831344</v>
       </c>
       <c r="W17" t="n">
-        <v>0</v>
+        <v>0.05060641025641319</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>33.10104821803127</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>2.760721285907529</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>26.31533333333485</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AB17" t="n">
-        <v>0</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC17" t="n">
-        <v>0</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD17" t="n">
-        <v>0</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE17" t="n">
-        <v>0</v>
+        <v>34.48025856044924</v>
       </c>
       <c r="AF17" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AG17" t="n">
-        <v>0</v>
+        <v>7.544914345831343</v>
       </c>
       <c r="AH17" t="n">
-        <v>0</v>
+        <v>33.10104821803127</v>
       </c>
       <c r="AI17" t="n">
-        <v>0</v>
+        <v>7.66227968009983</v>
       </c>
       <c r="AJ17" t="n">
         <v>46.512</v>
       </c>
-      <c r="AK17" t="inlineStr"/>
+      <c r="AK17" t="n">
+        <v>0</v>
+      </c>
       <c r="AL17" t="n">
-        <v>-1317.21984</v>
-      </c>
-      <c r="AM17" t="inlineStr"/>
+        <v>29.82137058919075</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>5.96427411783815</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>2.760721285907528</v>
+      </c>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2671,31 +2907,31 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21.4067760942761</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>21.4067760942761</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>16.33999999999695</v>
       </c>
       <c r="F18" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>16.33999999999695</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
@@ -2713,68 +2949,80 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>67.32000000000002</v>
+        <v>129.0644000000032</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>25.47589098532159</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="n">
-        <v>5.926331145149527</v>
+        <v>11.85266229029905</v>
       </c>
       <c r="U18" t="n">
-        <v>0.02112774026791275</v>
+        <v>0.04225548053582551</v>
       </c>
       <c r="V18" t="n">
-        <v>5.926331145149527</v>
+        <v>11.85266229029905</v>
       </c>
       <c r="W18" t="n">
-        <v>1025.994288926398</v>
+        <v>0.07949999999999413</v>
       </c>
       <c r="X18" t="n">
-        <v>26</v>
+        <v>51.99999999999617</v>
       </c>
       <c r="Y18" t="n">
-        <v>2.168473728106755</v>
+        <v>4.336947456213192</v>
       </c>
       <c r="Z18" t="n">
-        <v>20.67</v>
+        <v>41.33999999999695</v>
       </c>
       <c r="AA18" t="n">
-        <v>18.06458333333334</v>
+        <v>52</v>
       </c>
       <c r="AB18" t="n">
-        <v>2867.394179894181</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC18" t="n">
-        <v>27.08333333333335</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD18" t="n">
-        <v>15.38825757575758</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE18" t="n">
-        <v>27.08333333333334</v>
+        <v>54.16666666666669</v>
       </c>
       <c r="AF18" t="n">
-        <v>0</v>
+        <v>0.09999999999999987</v>
       </c>
       <c r="AG18" t="n">
-        <v>5.926331145149527</v>
+        <v>11.85266229029905</v>
       </c>
       <c r="AH18" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="AI18" t="n">
-        <v>6.018518518518518</v>
+        <v>12.03703703703704</v>
       </c>
       <c r="AJ18" t="n">
         <v>44.08</v>
       </c>
-      <c r="AK18" t="inlineStr"/>
+      <c r="AK18" t="n">
+        <v>991.8582445194642</v>
+      </c>
       <c r="AL18" t="n">
+        <v>34.19612794612795</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>6.839225589225591</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>4.336947456213191</v>
+      </c>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="n">
         <v>-0</v>
       </c>
-      <c r="AM18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2786,13 +3034,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>42.8135521885522</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>16.34</v>
+        <v>16.33999999999698</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2801,16 +3049,16 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>16.34</v>
+        <v>16.33999999999698</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
@@ -2828,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>83.66000000000003</v>
+        <v>145.4044000000002</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>10.30922431865884</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="n">
@@ -2844,34 +3092,34 @@
         <v>11.85266229029905</v>
       </c>
       <c r="W19" t="n">
-        <v>985.7165778527975</v>
+        <v>0.0794999999999942</v>
       </c>
       <c r="X19" t="n">
-        <v>52</v>
+        <v>51.99999999999621</v>
       </c>
       <c r="Y19" t="n">
-        <v>4.336947456213511</v>
+        <v>4.336947456213196</v>
       </c>
       <c r="Z19" t="n">
-        <v>41.34</v>
+        <v>41.33999999999698</v>
       </c>
       <c r="AA19" t="n">
-        <v>36.12916666666668</v>
+        <v>52.00000000000001</v>
       </c>
       <c r="AB19" t="n">
-        <v>5734.788359788363</v>
+        <v>8888.888888888891</v>
       </c>
       <c r="AC19" t="n">
-        <v>54.16666666666669</v>
+        <v>39.00000000000002</v>
       </c>
       <c r="AD19" t="n">
-        <v>30.77651515151516</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE19" t="n">
         <v>54.16666666666669</v>
       </c>
       <c r="AF19" t="n">
-        <v>0</v>
+        <v>0.09999999999999987</v>
       </c>
       <c r="AG19" t="n">
         <v>11.85266229029905</v>
@@ -2885,11 +3133,23 @@
       <c r="AJ19" t="n">
         <v>21.888</v>
       </c>
-      <c r="AK19" t="inlineStr"/>
+      <c r="AK19" t="n">
+        <v>969.6662445194643</v>
+      </c>
       <c r="AL19" t="n">
+        <v>34.19612794612796</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>6.839225589225592</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>4.336947456213195</v>
+      </c>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="n">
         <v>-0</v>
       </c>
-      <c r="AM19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2901,31 +3161,31 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>21.4067760942761</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>21.4067760942761</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>12.63280000000061</v>
       </c>
       <c r="F20" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>4.330000000000002</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>12.63280000000061</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>10.30922431865909</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>10.30922431865909</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
@@ -2943,68 +3203,80 @@
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>79.33000000000003</v>
+        <v>158.0372000000008</v>
       </c>
       <c r="R20" t="n">
         <v>0</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="n">
-        <v>5.926331145149527</v>
+        <v>10.78976462115079</v>
       </c>
       <c r="U20" t="n">
-        <v>0.02112774026791275</v>
+        <v>0.03846618403262313</v>
       </c>
       <c r="V20" t="n">
-        <v>5.926331145149527</v>
+        <v>10.78976462115079</v>
       </c>
       <c r="W20" t="n">
-        <v>985.2582889263988</v>
+        <v>0.07237076923077039</v>
       </c>
       <c r="X20" t="n">
-        <v>26</v>
+        <v>47.33685534591272</v>
       </c>
       <c r="Y20" t="n">
-        <v>2.168473728106755</v>
+        <v>3.94802796880006</v>
       </c>
       <c r="Z20" t="n">
-        <v>20.67</v>
+        <v>37.63280000000061</v>
       </c>
       <c r="AA20" t="n">
-        <v>18.06458333333334</v>
+        <v>52</v>
       </c>
       <c r="AB20" t="n">
-        <v>2867.394179894181</v>
+        <v>8888.888888888889</v>
       </c>
       <c r="AC20" t="n">
-        <v>27.08333333333335</v>
+        <v>39.00000000000001</v>
       </c>
       <c r="AD20" t="n">
-        <v>15.38825757575758</v>
+        <v>22.15909090909092</v>
       </c>
       <c r="AE20" t="n">
-        <v>27.08333333333334</v>
+        <v>49.3092243186591</v>
       </c>
       <c r="AF20" t="n">
-        <v>0</v>
+        <v>0.09999999999999987</v>
       </c>
       <c r="AG20" t="n">
-        <v>5.926331145149527</v>
+        <v>10.78976462115079</v>
       </c>
       <c r="AH20" t="n">
-        <v>26</v>
+        <v>47.33685534591272</v>
       </c>
       <c r="AI20" t="n">
-        <v>6.018518518518518</v>
+        <v>10.95760540414646</v>
       </c>
       <c r="AJ20" t="n">
         <v>3.344</v>
       </c>
-      <c r="AK20" t="inlineStr"/>
+      <c r="AK20" t="n">
+        <v>951.1331630467366</v>
+      </c>
       <c r="AL20" t="n">
+        <v>33.11669631323738</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>6.623339262647476</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>3.948027968800059</v>
+      </c>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="n">
         <v>-0</v>
       </c>
-      <c r="AM20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -3025,16 +3297,16 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>25</v>
+        <v>8.037200000000368</v>
       </c>
       <c r="G21" t="n">
-        <v>25</v>
+        <v>8.037200000000368</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>6.3682392692499e-13</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -3043,83 +3315,95 @@
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>6.3682392692499e-13</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>29.78448052676228</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>29.78448052676228</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>54.33000000000003</v>
+        <v>150.0000000000004</v>
       </c>
       <c r="R21" t="n">
         <v>0</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>4.863433476000979</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>0.01733844376470937</v>
       </c>
       <c r="V21" t="n">
-        <v>0</v>
+        <v>4.863433476000979</v>
       </c>
       <c r="W21" t="n">
-        <v>0</v>
+        <v>0.03262076923076852</v>
       </c>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>21.33685534591149</v>
       </c>
       <c r="Y21" t="n">
-        <v>0</v>
+        <v>1.779554240693202</v>
       </c>
       <c r="Z21" t="n">
-        <v>0</v>
+        <v>16.96279999999963</v>
       </c>
       <c r="AA21" t="n">
-        <v>0</v>
+        <v>29.6345213137668</v>
       </c>
       <c r="AB21" t="n">
-        <v>0</v>
+        <v>5065.730139105436</v>
       </c>
       <c r="AC21" t="n">
-        <v>0</v>
+        <v>22.22589098532511</v>
       </c>
       <c r="AD21" t="n">
-        <v>0</v>
+        <v>12.6283471507529</v>
       </c>
       <c r="AE21" t="n">
-        <v>0</v>
+        <v>22.22589098532447</v>
       </c>
       <c r="AF21" t="n">
-        <v>0</v>
+        <v>0.09999999999999987</v>
       </c>
       <c r="AG21" t="n">
-        <v>0</v>
+        <v>4.863433476000979</v>
       </c>
       <c r="AH21" t="n">
-        <v>0</v>
+        <v>21.33685534591149</v>
       </c>
       <c r="AI21" t="n">
-        <v>0</v>
+        <v>4.939086885627659</v>
       </c>
       <c r="AJ21" t="n">
         <v>0</v>
       </c>
-      <c r="AK21" t="inlineStr"/>
+      <c r="AK21" t="n">
+        <v>0</v>
+      </c>
       <c r="AL21" t="n">
+        <v>17.56743403638056</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>3.513486807276113</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>1.779554240693201</v>
+      </c>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="n">
         <v>-0</v>
       </c>
-      <c r="AM21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -3140,16 +3424,16 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>25</v>
+        <v>25.00000000000011</v>
       </c>
       <c r="G22" t="n">
-        <v>25</v>
+        <v>25.00000000000011</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1.457439833306946e-13</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -3158,47 +3442,47 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>1.457439833306946e-13</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>0.09999999999999955</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>0.09999999999999955</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>29.33000000000003</v>
+        <v>125.0000000000003</v>
       </c>
       <c r="R22" t="n">
         <v>0</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>-3.189146243560057e-14</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>-1.136950532463478e-16</v>
       </c>
       <c r="V22" t="n">
-        <v>0</v>
+        <v>-3.189146243560057e-14</v>
       </c>
       <c r="W22" t="n">
-        <v>0</v>
+        <v>-2.139073232268963e-16</v>
       </c>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>-1.399142239974668e-13</v>
       </c>
       <c r="Y22" t="n">
-        <v>0</v>
+        <v>-1.166924303565194e-14</v>
       </c>
       <c r="Z22" t="n">
-        <v>0</v>
+        <v>-1.112318080779861e-13</v>
       </c>
       <c r="AA22" t="n">
         <v>0</v>
@@ -3213,28 +3497,40 @@
         <v>0</v>
       </c>
       <c r="AE22" t="n">
-        <v>0</v>
+        <v>-1.457439833306946e-13</v>
       </c>
       <c r="AF22" t="n">
-        <v>0</v>
+        <v>0.09999999999999987</v>
       </c>
       <c r="AG22" t="n">
-        <v>0</v>
+        <v>-3.189146243560057e-14</v>
       </c>
       <c r="AH22" t="n">
-        <v>0</v>
+        <v>-1.399142239974668e-13</v>
       </c>
       <c r="AI22" t="n">
-        <v>0</v>
+        <v>-3.238755185126545e-14</v>
       </c>
       <c r="AJ22" t="n">
         <v>0</v>
       </c>
-      <c r="AK22" t="inlineStr"/>
+      <c r="AK22" t="n">
+        <v>0</v>
+      </c>
       <c r="AL22" t="n">
+        <v>-3.238755185126545e-14</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>-6.477510370253091e-15</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>-1.166924303565194e-14</v>
+      </c>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="n">
         <v>-0</v>
       </c>
-      <c r="AM22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -3288,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>4.330000000000027</v>
+        <v>100.0000000000003</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -3345,11 +3641,23 @@
       <c r="AJ23" t="n">
         <v>0</v>
       </c>
-      <c r="AK23" t="inlineStr"/>
+      <c r="AK23" t="n">
+        <v>0</v>
+      </c>
       <c r="AL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="n">
         <v>-0</v>
       </c>
-      <c r="AM23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -3361,19 +3669,19 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>21.40677609427609</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>21.40677609427609</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>4.330000000000013</v>
+        <v>25</v>
       </c>
       <c r="G24" t="n">
-        <v>4.330000000000013</v>
+        <v>25</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -3403,68 +3711,80 @@
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>75.00000000000028</v>
       </c>
       <c r="R24" t="n">
         <v>0</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="n">
-        <v>5.926331145149526</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
-        <v>0.02112774026791275</v>
+        <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>5.926331145149526</v>
+        <v>0</v>
       </c>
       <c r="W24" t="n">
-        <v>981.9142889263987</v>
+        <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>25.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="Y24" t="n">
-        <v>2.168473728106755</v>
+        <v>0</v>
       </c>
       <c r="Z24" t="n">
-        <v>20.66999999999999</v>
+        <v>0</v>
       </c>
       <c r="AA24" t="n">
-        <v>18.06458333333333</v>
+        <v>0</v>
       </c>
       <c r="AB24" t="n">
-        <v>2867.39417989418</v>
+        <v>0</v>
       </c>
       <c r="AC24" t="n">
-        <v>27.08333333333333</v>
+        <v>0</v>
       </c>
       <c r="AD24" t="n">
-        <v>15.38825757575757</v>
+        <v>0</v>
       </c>
       <c r="AE24" t="n">
-        <v>27.08333333333333</v>
+        <v>0</v>
       </c>
       <c r="AF24" t="n">
         <v>0</v>
       </c>
       <c r="AG24" t="n">
-        <v>5.926331145149525</v>
+        <v>0</v>
       </c>
       <c r="AH24" t="n">
-        <v>25.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="AI24" t="n">
-        <v>6.018518518518515</v>
+        <v>0</v>
       </c>
       <c r="AJ24" t="n">
         <v>0</v>
       </c>
-      <c r="AK24" t="inlineStr"/>
+      <c r="AK24" t="n">
+        <v>1000</v>
+      </c>
       <c r="AL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="n">
         <v>-0</v>
       </c>
-      <c r="AM24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -3476,19 +3796,19 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -3518,68 +3838,80 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>50.00000000000028</v>
       </c>
       <c r="R25" t="n">
         <v>0</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="n">
-        <v>7.167792870282449</v>
+        <v>-1.238503395557304e-15</v>
       </c>
       <c r="U25" t="n">
-        <v>0.02555362877106043</v>
+        <v>-4.415341873644577e-18</v>
       </c>
       <c r="V25" t="n">
-        <v>7.167792870282449</v>
+        <v>-1.238503395557304e-15</v>
       </c>
       <c r="W25" t="n">
-        <v>978.1256518219627</v>
+        <v>-8.307080513665876e-18</v>
       </c>
       <c r="X25" t="n">
-        <v>31.44654088050315</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="Y25" t="n">
-        <v>2.62273068227716</v>
+        <v>-4.531744868214346e-16</v>
       </c>
       <c r="Z25" t="n">
-        <v>25</v>
+        <v>-4.319681867106255e-15</v>
       </c>
       <c r="AA25" t="n">
-        <v>21.84879454926626</v>
+        <v>-7.546614023595834e-15</v>
       </c>
       <c r="AB25" t="n">
-        <v>3468.06262686766</v>
+        <v>-1.290019491212963e-12</v>
       </c>
       <c r="AC25" t="n">
-        <v>32.75681341719079</v>
+        <v>-5.659960517696877e-15</v>
       </c>
       <c r="AD25" t="n">
-        <v>18.61182580522204</v>
+        <v>-3.215886657782316e-15</v>
       </c>
       <c r="AE25" t="n">
-        <v>32.75681341719079</v>
+        <v>-5.659960517696878e-15</v>
       </c>
       <c r="AF25" t="n">
-        <v>0</v>
+        <v>-1.0449157878825e-17</v>
       </c>
       <c r="AG25" t="n">
-        <v>7.167792870282448</v>
+        <v>-1.238503395557303e-15</v>
       </c>
       <c r="AH25" t="n">
-        <v>31.44654088050315</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="AI25" t="n">
-        <v>7.27929187048684</v>
+        <v>-1.257769003932639e-15</v>
       </c>
       <c r="AJ25" t="n">
         <v>0</v>
       </c>
-      <c r="AK25" t="inlineStr"/>
+      <c r="AK25" t="n">
+        <v>1000</v>
+      </c>
       <c r="AL25" t="n">
+        <v>-4.473655661714955e-15</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>-8.947311323429911e-16</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>-4.531744868214346e-16</v>
+      </c>
+      <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="n">
         <v>-0</v>
       </c>
-      <c r="AM25" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -3591,19 +3923,19 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -3633,68 +3965,80 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>25.00000000000015</v>
       </c>
       <c r="R26" t="n">
         <v>0</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="n">
-        <v>7.167792870282449</v>
+        <v>-1.238503395557304e-15</v>
       </c>
       <c r="U26" t="n">
-        <v>0.02555362877106043</v>
+        <v>-4.415341873644577e-18</v>
       </c>
       <c r="V26" t="n">
-        <v>7.167792870282449</v>
+        <v>-1.238503395557304e-15</v>
       </c>
       <c r="W26" t="n">
-        <v>978.1256518219627</v>
+        <v>-8.307080513665876e-18</v>
       </c>
       <c r="X26" t="n">
-        <v>31.44654088050315</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="Y26" t="n">
-        <v>2.62273068227716</v>
+        <v>-4.531744868214346e-16</v>
       </c>
       <c r="Z26" t="n">
-        <v>25</v>
+        <v>-4.319681867106255e-15</v>
       </c>
       <c r="AA26" t="n">
-        <v>21.84879454926626</v>
+        <v>-7.546614023595834e-15</v>
       </c>
       <c r="AB26" t="n">
-        <v>3468.06262686766</v>
+        <v>-1.290019491212963e-12</v>
       </c>
       <c r="AC26" t="n">
-        <v>32.75681341719079</v>
+        <v>-5.659960517696877e-15</v>
       </c>
       <c r="AD26" t="n">
-        <v>18.61182580522204</v>
+        <v>-3.215886657782316e-15</v>
       </c>
       <c r="AE26" t="n">
-        <v>32.75681341719079</v>
+        <v>-5.659960517696878e-15</v>
       </c>
       <c r="AF26" t="n">
-        <v>0</v>
+        <v>-1.0449157878825e-17</v>
       </c>
       <c r="AG26" t="n">
-        <v>7.167792870282448</v>
+        <v>-1.238503395557303e-15</v>
       </c>
       <c r="AH26" t="n">
-        <v>31.44654088050315</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="AI26" t="n">
-        <v>7.27929187048684</v>
+        <v>-1.257769003932639e-15</v>
       </c>
       <c r="AJ26" t="n">
         <v>0</v>
       </c>
-      <c r="AK26" t="inlineStr"/>
+      <c r="AK26" t="n">
+        <v>1000</v>
+      </c>
       <c r="AL26" t="n">
+        <v>-4.473655661714955e-15</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>-8.947311323429911e-16</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>-4.531744868214346e-16</v>
+      </c>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="n">
         <v>-0</v>
       </c>
-      <c r="AM26" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3706,19 +4050,19 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>25.89111767570888</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>25.00000000000015</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>25.00000000000015</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -3755,61 +4099,73 @@
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="n">
-        <v>7.167792870282449</v>
+        <v>-4.358010037207033e-14</v>
       </c>
       <c r="U27" t="n">
-        <v>0.02555362877106043</v>
+        <v>-1.553657767275235e-16</v>
       </c>
       <c r="V27" t="n">
-        <v>7.167792870282449</v>
+        <v>-4.358010037207033e-14</v>
       </c>
       <c r="W27" t="n">
-        <v>978.1256518219627</v>
+        <v>-2.923071538463765e-16</v>
       </c>
       <c r="X27" t="n">
-        <v>31.44654088050315</v>
+        <v>-1.911946163523469e-13</v>
       </c>
       <c r="Y27" t="n">
-        <v>2.62273068227716</v>
+        <v>-1.594617317367364e-14</v>
       </c>
       <c r="Z27" t="n">
-        <v>25</v>
+        <v>-1.519997200001158e-13</v>
       </c>
       <c r="AA27" t="n">
-        <v>21.84879454926626</v>
+        <v>-2.655480782671485e-13</v>
       </c>
       <c r="AB27" t="n">
-        <v>3468.06262686766</v>
+        <v>-4.539283389182025e-11</v>
       </c>
       <c r="AC27" t="n">
-        <v>32.75681341719079</v>
+        <v>-1.991610587003614e-13</v>
       </c>
       <c r="AD27" t="n">
-        <v>18.61182580522204</v>
+        <v>-1.131596924433872e-13</v>
       </c>
       <c r="AE27" t="n">
-        <v>32.75681341719079</v>
+        <v>-1.991610587003614e-13</v>
       </c>
       <c r="AF27" t="n">
-        <v>0</v>
+        <v>-1.0449157878825e-17</v>
       </c>
       <c r="AG27" t="n">
-        <v>7.167792870282448</v>
+        <v>-4.358010037207033e-14</v>
       </c>
       <c r="AH27" t="n">
-        <v>31.44654088050315</v>
+        <v>-1.911946163523469e-13</v>
       </c>
       <c r="AI27" t="n">
-        <v>7.27929187048684</v>
+        <v>-4.425801304452475e-14</v>
       </c>
       <c r="AJ27" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" t="inlineStr"/>
+      <c r="AK27" t="n">
+        <v>1000</v>
+      </c>
       <c r="AL27" t="n">
+        <v>-1.574177054879119e-13</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>-3.148354109758239e-14</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>-1.594617317367363e-14</v>
+      </c>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="n">
         <v>-0</v>
       </c>
-      <c r="AM27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
export new output structure
</commit_message>
<xml_diff>
--- a/spine_projects/02_output_data/01_basic_energy_model_outputs/output_last_run.xlsx
+++ b/spine_projects/02_output_data/01_basic_energy_model_outputs/output_last_run.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Total costs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="flows_node_states" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="system_costs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ27"/>
+  <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,212 +437,197 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>timeseries</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow</t>
+          <t>connection_flow_pipeline_District_Heating_from_node_Waste_Heat</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.1</t>
+          <t>connection_flow.1_pipeline_District_Heating_to_node_District_Heating</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.2</t>
+          <t>connection_flow.2_pipeline_storage_e-methanol_from_node_E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.3</t>
+          <t>connection_flow.3_pipeline_storage_e-methanol_from_node_E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.4</t>
+          <t>connection_flow.4_pipeline_storage_e-methanol_to_node_E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.5</t>
+          <t>connection_flow.5_pipeline_storage_e-methanol_to_node_E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.6</t>
+          <t>connection_flow.6_pipeline_storage_hydrogen_from_node_Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.7</t>
+          <t>connection_flow.7_pipeline_storage_hydrogen_from_node_Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.8</t>
+          <t>connection_flow.8_pipeline_storage_hydrogen_to_node_Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.9</t>
+          <t>connection_flow.9_pipeline_storage_hydrogen_to_node_Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.10</t>
+          <t>connection_flow.10_power_line_Wholesale_Kasso_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.11</t>
+          <t>connection_flow.11_power_line_Wholesale_Kasso_from_node_Power_Wholesale</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.12</t>
+          <t>connection_flow.12_power_line_Wholesale_Kasso_to_node_Power_Kasso</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>connection_flow.13</t>
+          <t>connection_flow.13_power_line_Wholesale_Kasso_to_node_Power_Wholesale</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>node_state</t>
+          <t>node_state_E-Methanol_storage_Kasso__realisation</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>node_state.1</t>
+          <t>node_state.1_Hydrogen_storage_Kasso__realisation</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>total_costs</t>
+          <t>unit_flow_CO2_Vaporizer_from_node_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow</t>
+          <t>unit_flow.1_CO2_Vaporizer_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.1</t>
+          <t>unit_flow.2_CO2_Vaporizer_to_node_Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.2</t>
+          <t>unit_flow.3_Destilation_Tower_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.3</t>
+          <t>unit_flow.4_Destilation_Tower_from_node_Raw_Methanol</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.4</t>
+          <t>unit_flow.5_Destilation_Tower_from_node_Steam</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.5</t>
+          <t>unit_flow.6_Destilation_Tower_to_node_E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.6</t>
+          <t>unit_flow.7_Electrolyzer_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.7</t>
+          <t>unit_flow.8_Electrolyzer_from_node_Water</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.8</t>
+          <t>unit_flow.9_Electrolyzer_to_node_Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.9</t>
+          <t>unit_flow.10_Electrolyzer_to_node_Waste_Heat</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.10</t>
+          <t>unit_flow.11_Methanol_Reactor_from_node_Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.11</t>
+          <t>unit_flow.12_Methanol_Reactor_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.12</t>
+          <t>unit_flow.13_Methanol_Reactor_from_node_Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.13</t>
+          <t>unit_flow.14_Methanol_Reactor_to_node_Raw_Methanol</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.14</t>
+          <t>unit_flow.15_Methanol_Reactor_to_node_Waste_Heat</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.15</t>
+          <t>unit_flow.16_Solar_Plant_Kasso_to_node_Power_Kasso</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.16</t>
+          <t>unit_flow.17_Steam_Plant_from_node_Power_Kasso</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.17</t>
+          <t>unit_flow.18_Steam_Plant_from_node_Waste_Heat</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.18</t>
+          <t>unit_flow.19_Steam_Plant_from_node_Water</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.19</t>
+          <t>unit_flow.20_Steam_Plant_to_node_Steam</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>unit_flow.20</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>unit_flow_op</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>proceeds from PV</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>adjusted costs</t>
+          <t>Revenue_from_PV</t>
         </is>
       </c>
     </row>
@@ -736,7 +722,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>toy</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -751,7 +737,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -771,7 +757,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -791,7 +777,7 @@
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -816,12 +802,12 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Steam_Plant</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
@@ -839,18 +825,7 @@
           <t>Steam_Plant</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>Steam_Plant</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>Electrolyzer</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -929,7 +904,11 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
       <c r="T3" t="inlineStr">
         <is>
           <t>from_node</t>
@@ -937,111 +916,100 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>to_node</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
         <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>to_node</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>to_node</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>from_node</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>from_node</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>to_node</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>to_node</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>to_node</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>to_node</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>to_node</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AN3" t="inlineStr">
-        <is>
-          <t>to_node</t>
-        </is>
-      </c>
-      <c r="AO3" t="inlineStr">
-        <is>
-          <t>from_node</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1128,119 +1096,112 @@
           <t>realisation</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Carbon_Dioxide</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
+          <t>Vaporized_Carbon_Dioxide</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
           <t>Power_Kasso</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Raw_Methanol</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Steam</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
         <is>
           <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Raw_Methanol</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>Power_Kasso</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>Steam</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>Vaporized_Carbon_Dioxide</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-      <c r="AN4" t="inlineStr">
-        <is>
-          <t>Steam</t>
-        </is>
-      </c>
-      <c r="AO4" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1300,77 +1261,70 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-94427.62279218005</v>
+        <v>7.167792870282449</v>
       </c>
       <c r="T5" t="n">
+        <v>0.02555362877106042</v>
+      </c>
+      <c r="U5" t="n">
         <v>7.167792870282449</v>
       </c>
-      <c r="U5" t="n">
-        <v>0.02555362877106042</v>
-      </c>
       <c r="V5" t="n">
-        <v>7.167792870282449</v>
+        <v>0.04807692307692308</v>
       </c>
       <c r="W5" t="n">
-        <v>0.04807692307692308</v>
+        <v>31.44654088050315</v>
       </c>
       <c r="X5" t="n">
+        <v>2.62273068227716</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>43.67575122292104</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>7465.940379986502</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>32.75681341719078</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>18.61182580522204</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>32.75681341719079</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>7.167792870282448</v>
+      </c>
+      <c r="AG5" t="n">
         <v>31.44654088050315</v>
       </c>
-      <c r="Y5" t="n">
-        <v>2.62273068227716</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>25</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>43.67575122292104</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>7465.940379986502</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>32.75681341719078</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>18.61182580522204</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>32.75681341719079</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>7.167792870282448</v>
-      </c>
       <c r="AH5" t="n">
-        <v>31.44654088050315</v>
+        <v>7.27929187048684</v>
       </c>
       <c r="AI5" t="n">
-        <v>7.27929187048684</v>
+        <v>0</v>
       </c>
       <c r="AJ5" t="n">
         <v>0</v>
       </c>
       <c r="AK5" t="n">
-        <v>0</v>
+        <v>25.89111767570888</v>
       </c>
       <c r="AL5" t="n">
-        <v>25.89111767570888</v>
+        <v>5.178223535141776</v>
       </c>
       <c r="AM5" t="n">
-        <v>5.178223535141776</v>
+        <v>2.622730682277159</v>
       </c>
       <c r="AN5" t="n">
-        <v>2.622730682277159</v>
-      </c>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="n">
         <v>-0</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>-94427.62279218005</v>
       </c>
     </row>
     <row r="6">
@@ -1430,75 +1384,72 @@
       <c r="R6" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>1.241461725132921</v>
+      </c>
       <c r="T6" t="n">
+        <v>0.004425888503147669</v>
+      </c>
+      <c r="U6" t="n">
         <v>1.241461725132921</v>
       </c>
-      <c r="U6" t="n">
-        <v>0.004425888503147669</v>
-      </c>
       <c r="V6" t="n">
+        <v>0.008326923076923084</v>
+      </c>
+      <c r="W6" t="n">
+        <v>5.44654088050315</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.4542569541704045</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>4.330000000000004</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>7.56464011180993</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1293.100873813663</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>5.673480083857449</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>3.22356822946446</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>5.67348008385745</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF6" t="n">
         <v>1.241461725132921</v>
       </c>
-      <c r="W6" t="n">
-        <v>0.008326923076923084</v>
-      </c>
-      <c r="X6" t="n">
+      <c r="AG6" t="n">
         <v>5.44654088050315</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AH6" t="n">
+        <v>1.260773351968322</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>4.484341581432782</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.8968683162865564</v>
+      </c>
+      <c r="AM6" t="n">
         <v>0.4542569541704045</v>
       </c>
-      <c r="Z6" t="n">
-        <v>4.330000000000004</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>7.56464011180993</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1293.100873813663</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>5.673480083857449</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>3.22356822946446</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>5.67348008385745</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>1.241461725132921</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>5.44654088050315</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>1.260773351968322</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>4.484341581432782</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0.8968683162865564</v>
-      </c>
       <c r="AN6" t="n">
-        <v>0.4542569541704045</v>
-      </c>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1557,75 +1508,72 @@
       <c r="R7" t="n">
         <v>11.91666666666667</v>
       </c>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>5.926331145149526</v>
+      </c>
       <c r="T7" t="n">
+        <v>0.02112774026791275</v>
+      </c>
+      <c r="U7" t="n">
         <v>5.926331145149526</v>
       </c>
-      <c r="U7" t="n">
-        <v>0.02112774026791275</v>
-      </c>
       <c r="V7" t="n">
+        <v>0.03974999999999999</v>
+      </c>
+      <c r="W7" t="n">
+        <v>26</v>
+      </c>
+      <c r="X7" t="n">
+        <v>2.168473728106755</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>20.66999999999999</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>51.99999999999999</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>8888.888888888887</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>22.15909090909091</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>27.08333333333334</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF7" t="n">
         <v>5.926331145149526</v>
       </c>
-      <c r="W7" t="n">
-        <v>0.03974999999999999</v>
-      </c>
-      <c r="X7" t="n">
+      <c r="AG7" t="n">
         <v>26</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AH7" t="n">
+        <v>6.018518518518517</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>947.839122259732</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>28.17760942760943</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>5.635521885521886</v>
+      </c>
+      <c r="AM7" t="n">
         <v>2.168473728106755</v>
       </c>
-      <c r="Z7" t="n">
-        <v>20.66999999999999</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>51.99999999999999</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>8888.888888888887</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>39</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>22.15909090909091</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>27.08333333333334</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>5.926331145149526</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>26</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>6.018518518518517</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>947.839122259732</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>28.17760942760943</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>5.635521885521886</v>
-      </c>
       <c r="AN7" t="n">
-        <v>2.168473728106755</v>
-      </c>
-      <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1684,75 +1632,72 @@
       <c r="R8" t="n">
         <v>0</v>
       </c>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="n">
+        <v>11.1415025528811</v>
+      </c>
       <c r="T8" t="n">
+        <v>0.03972015170367595</v>
+      </c>
+      <c r="U8" t="n">
         <v>11.1415025528811</v>
       </c>
-      <c r="U8" t="n">
-        <v>0.03972015170367595</v>
-      </c>
       <c r="V8" t="n">
+        <v>0.07472999999999994</v>
+      </c>
+      <c r="W8" t="n">
+        <v>48.87999999999996</v>
+      </c>
+      <c r="X8" t="n">
+        <v>4.076730608840697</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>38.85959999999996</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>51.99999999999994</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>8888.888888888878</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>38.99999999999996</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>22.15909090909089</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>50.91666666666664</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF8" t="n">
         <v>11.1415025528811</v>
       </c>
-      <c r="W8" t="n">
-        <v>0.07472999999999994</v>
-      </c>
-      <c r="X8" t="n">
+      <c r="AG8" t="n">
         <v>48.87999999999996</v>
       </c>
-      <c r="Y8" t="n">
-        <v>4.076730608840697</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>38.85959999999996</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>51.99999999999994</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>8888.888888888878</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>38.99999999999996</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>22.15909090909089</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>50.91666666666664</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>11.1415025528811</v>
-      </c>
       <c r="AH8" t="n">
-        <v>48.87999999999996</v>
+        <v>11.3148148148148</v>
       </c>
       <c r="AI8" t="n">
-        <v>11.3148148148148</v>
+        <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0</v>
+        <v>947.7855498482963</v>
       </c>
       <c r="AK8" t="n">
-        <v>947.7855498482963</v>
+        <v>33.47390572390569</v>
       </c>
       <c r="AL8" t="n">
-        <v>33.47390572390569</v>
+        <v>6.694781144781139</v>
       </c>
       <c r="AM8" t="n">
-        <v>6.694781144781139</v>
+        <v>4.076730608840696</v>
       </c>
       <c r="AN8" t="n">
-        <v>4.076730608840696</v>
-      </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1811,75 +1756,72 @@
       <c r="R9" t="n">
         <v>0</v>
       </c>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>8.53391684901532</v>
+      </c>
       <c r="T9" t="n">
+        <v>0.03042394598579437</v>
+      </c>
+      <c r="U9" t="n">
         <v>8.53391684901532</v>
       </c>
-      <c r="U9" t="n">
-        <v>0.03042394598579437</v>
-      </c>
       <c r="V9" t="n">
-        <v>8.53391684901532</v>
+        <v>0.05723999999999999</v>
       </c>
       <c r="W9" t="n">
-        <v>0.05723999999999999</v>
+        <v>37.44</v>
       </c>
       <c r="X9" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>29.76479999999999</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>8.533916849015318</v>
+      </c>
+      <c r="AG9" t="n">
         <v>37.44</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AH9" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>947.8123360540142</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>30.82575757575758</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>6.165151515151517</v>
+      </c>
+      <c r="AM9" t="n">
         <v>3.122602168473728</v>
       </c>
-      <c r="Z9" t="n">
-        <v>29.76479999999999</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>8.533916849015318</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>37.44</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>8.666666666666666</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>947.8123360540142</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>30.82575757575758</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>6.165151515151517</v>
-      </c>
       <c r="AN9" t="n">
-        <v>3.122602168473728</v>
-      </c>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1938,75 +1880,72 @@
       <c r="R10" t="n">
         <v>0</v>
       </c>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>8.53391684901532</v>
+      </c>
       <c r="T10" t="n">
+        <v>0.03042394598579437</v>
+      </c>
+      <c r="U10" t="n">
         <v>8.53391684901532</v>
       </c>
-      <c r="U10" t="n">
-        <v>0.03042394598579437</v>
-      </c>
       <c r="V10" t="n">
-        <v>8.53391684901532</v>
+        <v>0.05723999999999999</v>
       </c>
       <c r="W10" t="n">
-        <v>0.05723999999999999</v>
+        <v>37.44</v>
       </c>
       <c r="X10" t="n">
+        <v>3.122602168473728</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>29.76479999999999</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>8.533916849015318</v>
+      </c>
+      <c r="AG10" t="n">
         <v>37.44</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AH10" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>947.8123360540142</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>30.82575757575758</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>6.165151515151517</v>
+      </c>
+      <c r="AM10" t="n">
         <v>3.122602168473728</v>
       </c>
-      <c r="Z10" t="n">
-        <v>29.76479999999999</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG10" t="n">
-        <v>8.533916849015318</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>37.44</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>8.666666666666666</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>947.8123360540142</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>30.82575757575758</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>6.165151515151517</v>
-      </c>
       <c r="AN10" t="n">
-        <v>3.122602168473728</v>
-      </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -2065,75 +2004,72 @@
       <c r="R11" t="n">
         <v>14.08333333333465</v>
       </c>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="n">
+        <v>5.452224653537774</v>
+      </c>
       <c r="T11" t="n">
+        <v>0.01943752104648048</v>
+      </c>
+      <c r="U11" t="n">
         <v>5.452224653537774</v>
       </c>
-      <c r="U11" t="n">
-        <v>0.01943752104648048</v>
-      </c>
       <c r="V11" t="n">
-        <v>5.452224653537774</v>
+        <v>0.0365700000000014</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0365700000000014</v>
+        <v>23.92000000000091</v>
       </c>
       <c r="X11" t="n">
+        <v>1.994995829858291</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>19.01640000000073</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>24.91666666666763</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>5.452224653537773</v>
+      </c>
+      <c r="AG11" t="n">
         <v>23.92000000000091</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AH11" t="n">
+        <v>5.537037037037249</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>947.8439924789535</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>27.69612794612816</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>5.539225589225634</v>
+      </c>
+      <c r="AM11" t="n">
         <v>1.994995829858291</v>
       </c>
-      <c r="Z11" t="n">
-        <v>19.01640000000073</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>24.91666666666763</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>5.452224653537773</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>23.92000000000091</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>5.537037037037249</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>947.8439924789535</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>27.69612794612816</v>
-      </c>
-      <c r="AM11" t="n">
-        <v>5.539225589225634</v>
-      </c>
       <c r="AN11" t="n">
-        <v>1.994995829858291</v>
-      </c>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -2192,75 +2128,72 @@
       <c r="R12" t="n">
         <v>28.16666666666718</v>
       </c>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="n">
+        <v>5.452224653537741</v>
+      </c>
       <c r="T12" t="n">
+        <v>0.01943752104648036</v>
+      </c>
+      <c r="U12" t="n">
         <v>5.452224653537741</v>
       </c>
-      <c r="U12" t="n">
-        <v>0.01943752104648036</v>
-      </c>
       <c r="V12" t="n">
+        <v>0.03657000000000117</v>
+      </c>
+      <c r="W12" t="n">
+        <v>23.92000000000077</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1.994995829858279</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>19.01640000000061</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>24.91666666666747</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF12" t="n">
         <v>5.452224653537741</v>
       </c>
-      <c r="W12" t="n">
-        <v>0.03657000000000117</v>
-      </c>
-      <c r="X12" t="n">
+      <c r="AG12" t="n">
         <v>23.92000000000077</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AH12" t="n">
+        <v>5.537037037037215</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>947.8439924789535</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>27.69612794612813</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>5.539225589225627</v>
+      </c>
+      <c r="AM12" t="n">
         <v>1.994995829858279</v>
       </c>
-      <c r="Z12" t="n">
-        <v>19.01640000000061</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>24.91666666666747</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>5.452224653537741</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>23.92000000000077</v>
-      </c>
-      <c r="AI12" t="n">
-        <v>5.537037037037215</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>947.8439924789535</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>27.69612794612813</v>
-      </c>
-      <c r="AM12" t="n">
-        <v>5.539225589225627</v>
-      </c>
       <c r="AN12" t="n">
-        <v>1.994995829858279</v>
-      </c>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -2319,75 +2252,72 @@
       <c r="R13" t="n">
         <v>15.16666666666668</v>
       </c>
-      <c r="S13" t="inlineStr"/>
+      <c r="S13" t="n">
+        <v>11.3785557986872</v>
+      </c>
       <c r="T13" t="n">
+        <v>0.04056526131439287</v>
+      </c>
+      <c r="U13" t="n">
         <v>11.3785557986872</v>
       </c>
-      <c r="U13" t="n">
-        <v>0.04056526131439287</v>
-      </c>
       <c r="V13" t="n">
+        <v>0.07632000000000072</v>
+      </c>
+      <c r="W13" t="n">
+        <v>49.92000000000047</v>
+      </c>
+      <c r="X13" t="n">
+        <v>4.16346955796501</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>39.68640000000037</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>52.0000000000005</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF13" t="n">
         <v>11.3785557986872</v>
       </c>
-      <c r="W13" t="n">
-        <v>0.07632000000000072</v>
-      </c>
-      <c r="X13" t="n">
+      <c r="AG13" t="n">
         <v>49.92000000000047</v>
       </c>
-      <c r="Y13" t="n">
-        <v>4.16346955796501</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>39.68640000000037</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>52.0000000000005</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>11.3785557986872</v>
-      </c>
       <c r="AH13" t="n">
-        <v>49.92000000000047</v>
+        <v>11.55555555555566</v>
       </c>
       <c r="AI13" t="n">
-        <v>11.55555555555566</v>
+        <v>0</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0</v>
+        <v>947.7831147386855</v>
       </c>
       <c r="AK13" t="n">
-        <v>947.7831147386855</v>
+        <v>33.71464646464658</v>
       </c>
       <c r="AL13" t="n">
-        <v>33.71464646464658</v>
+        <v>6.742929292929316</v>
       </c>
       <c r="AM13" t="n">
-        <v>6.742929292929316</v>
+        <v>4.163469557965009</v>
       </c>
       <c r="AN13" t="n">
-        <v>4.163469557965009</v>
-      </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -2446,75 +2376,72 @@
       <c r="R14" t="n">
         <v>0</v>
       </c>
-      <c r="S14" t="inlineStr"/>
+      <c r="S14" t="n">
+        <v>11.85266229029905</v>
+      </c>
       <c r="T14" t="n">
+        <v>0.04225548053582551</v>
+      </c>
+      <c r="U14" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="U14" t="n">
-        <v>0.04225548053582551</v>
-      </c>
       <c r="V14" t="n">
+        <v>0.0795</v>
+      </c>
+      <c r="W14" t="n">
+        <v>52</v>
+      </c>
+      <c r="X14" t="n">
+        <v>4.336947456213511</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>41.34</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>52.00000000000001</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>8888.888888888891</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>39.00000000000002</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>54.16666666666669</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF14" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="W14" t="n">
-        <v>0.0795</v>
-      </c>
-      <c r="X14" t="n">
+      <c r="AG14" t="n">
         <v>52</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AH14" t="n">
+        <v>12.03703703703704</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>5.168</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>952.9462445194641</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>34.19612794612796</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>6.839225589225592</v>
+      </c>
+      <c r="AM14" t="n">
         <v>4.336947456213511</v>
       </c>
-      <c r="Z14" t="n">
-        <v>41.34</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>52.00000000000001</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>8888.888888888891</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>39.00000000000002</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>54.16666666666669</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG14" t="n">
-        <v>11.85266229029905</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>52</v>
-      </c>
-      <c r="AI14" t="n">
-        <v>12.03703703703704</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>5.168</v>
-      </c>
-      <c r="AK14" t="n">
-        <v>952.9462445194641</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>34.19612794612796</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>6.839225589225592</v>
-      </c>
       <c r="AN14" t="n">
-        <v>4.336947456213511</v>
-      </c>
-      <c r="AO14" t="inlineStr"/>
-      <c r="AP14" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2573,75 +2500,72 @@
       <c r="R15" t="n">
         <v>4.519741439550772</v>
       </c>
-      <c r="S15" t="inlineStr"/>
+      <c r="S15" t="n">
+        <v>7.544914345831342</v>
+      </c>
       <c r="T15" t="n">
+        <v>0.02689809035947002</v>
+      </c>
+      <c r="U15" t="n">
         <v>7.544914345831342</v>
       </c>
-      <c r="U15" t="n">
-        <v>0.02689809035947002</v>
-      </c>
       <c r="V15" t="n">
-        <v>7.544914345831342</v>
+        <v>0.05060641025641316</v>
       </c>
       <c r="W15" t="n">
-        <v>0.05060641025641316</v>
+        <v>33.10104821803125</v>
       </c>
       <c r="X15" t="n">
+        <v>2.760721285907527</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>26.31533333333484</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>34.48025856044923</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>7.544914345831341</v>
+      </c>
+      <c r="AG15" t="n">
         <v>33.10104821803125</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AH15" t="n">
+        <v>7.662279680099826</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>31.008</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>978.8304954993843</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>29.82137058919074</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>5.964274117838149</v>
+      </c>
+      <c r="AM15" t="n">
         <v>2.760721285907527</v>
       </c>
-      <c r="Z15" t="n">
-        <v>26.31533333333484</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>34.48025856044923</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG15" t="n">
-        <v>7.544914345831341</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>33.10104821803125</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>7.662279680099826</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>31.008</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>978.8304954993843</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>29.82137058919074</v>
-      </c>
-      <c r="AM15" t="n">
-        <v>5.964274117838149</v>
-      </c>
       <c r="AN15" t="n">
-        <v>2.760721285907527</v>
-      </c>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2700,75 +2624,72 @@
       <c r="R16" t="n">
         <v>36.12281621243488</v>
       </c>
-      <c r="S16" t="inlineStr"/>
+      <c r="S16" t="n">
+        <v>1.618583200681815</v>
+      </c>
       <c r="T16" t="n">
+        <v>0.005770350091557274</v>
+      </c>
+      <c r="U16" t="n">
         <v>1.618583200681815</v>
       </c>
-      <c r="U16" t="n">
-        <v>0.005770350091557274</v>
-      </c>
       <c r="V16" t="n">
+        <v>0.01085641025641317</v>
+      </c>
+      <c r="W16" t="n">
+        <v>7.101048218031259</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.5922475578007722</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>5.64533333333485</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>7.396925227115897</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF16" t="n">
         <v>1.618583200681815</v>
       </c>
-      <c r="W16" t="n">
-        <v>0.01085641025641317</v>
-      </c>
-      <c r="X16" t="n">
+      <c r="AG16" t="n">
         <v>7.101048218031259</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AH16" t="n">
+        <v>1.64376116158131</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>51.072</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>23.80285207067223</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>4.760570414134445</v>
+      </c>
+      <c r="AM16" t="n">
         <v>0.5922475578007722</v>
       </c>
-      <c r="Z16" t="n">
-        <v>5.64533333333485</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>7.396925227115897</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>1.618583200681815</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>7.101048218031259</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>1.64376116158131</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>51.072</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>23.80285207067223</v>
-      </c>
-      <c r="AM16" t="n">
-        <v>4.760570414134445</v>
-      </c>
       <c r="AN16" t="n">
-        <v>0.5922475578007722</v>
-      </c>
-      <c r="AO16" t="inlineStr"/>
-      <c r="AP16" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2827,75 +2748,72 @@
       <c r="R17" t="n">
         <v>40.64255765198565</v>
       </c>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="n">
+        <v>7.544914345831344</v>
+      </c>
       <c r="T17" t="n">
+        <v>0.02689809035947004</v>
+      </c>
+      <c r="U17" t="n">
         <v>7.544914345831344</v>
       </c>
-      <c r="U17" t="n">
-        <v>0.02689809035947004</v>
-      </c>
       <c r="V17" t="n">
-        <v>7.544914345831344</v>
+        <v>0.05060641025641319</v>
       </c>
       <c r="W17" t="n">
-        <v>0.05060641025641319</v>
+        <v>33.10104821803127</v>
       </c>
       <c r="X17" t="n">
+        <v>2.760721285907529</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>26.31533333333485</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>34.48025856044924</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>7.544914345831343</v>
+      </c>
+      <c r="AG17" t="n">
         <v>33.10104821803127</v>
       </c>
-      <c r="Y17" t="n">
-        <v>2.760721285907529</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>26.31533333333485</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>34.48025856044924</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AG17" t="n">
-        <v>7.544914345831343</v>
-      </c>
       <c r="AH17" t="n">
-        <v>33.10104821803127</v>
+        <v>7.66227968009983</v>
       </c>
       <c r="AI17" t="n">
-        <v>7.66227968009983</v>
+        <v>46.512</v>
       </c>
       <c r="AJ17" t="n">
-        <v>46.512</v>
+        <v>0</v>
       </c>
       <c r="AK17" t="n">
-        <v>0</v>
+        <v>29.82137058919075</v>
       </c>
       <c r="AL17" t="n">
-        <v>29.82137058919075</v>
+        <v>5.96427411783815</v>
       </c>
       <c r="AM17" t="n">
-        <v>5.96427411783815</v>
+        <v>2.760721285907528</v>
       </c>
       <c r="AN17" t="n">
-        <v>2.760721285907528</v>
-      </c>
-      <c r="AO17" t="inlineStr"/>
-      <c r="AP17" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2954,75 +2872,72 @@
       <c r="R18" t="n">
         <v>25.47589098532159</v>
       </c>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="n">
+        <v>11.85266229029905</v>
+      </c>
       <c r="T18" t="n">
+        <v>0.04225548053582551</v>
+      </c>
+      <c r="U18" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="U18" t="n">
-        <v>0.04225548053582551</v>
-      </c>
       <c r="V18" t="n">
+        <v>0.07949999999999413</v>
+      </c>
+      <c r="W18" t="n">
+        <v>51.99999999999617</v>
+      </c>
+      <c r="X18" t="n">
+        <v>4.336947456213192</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>41.33999999999695</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>54.16666666666669</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0.09999999999999987</v>
+      </c>
+      <c r="AF18" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="W18" t="n">
-        <v>0.07949999999999413</v>
-      </c>
-      <c r="X18" t="n">
-        <v>51.99999999999617</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>4.336947456213192</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>41.33999999999695</v>
-      </c>
-      <c r="AA18" t="n">
+      <c r="AG18" t="n">
         <v>52</v>
       </c>
-      <c r="AB18" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>54.16666666666669</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>0.09999999999999987</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>11.85266229029905</v>
-      </c>
       <c r="AH18" t="n">
-        <v>52</v>
+        <v>12.03703703703704</v>
       </c>
       <c r="AI18" t="n">
-        <v>12.03703703703704</v>
+        <v>44.08</v>
       </c>
       <c r="AJ18" t="n">
-        <v>44.08</v>
+        <v>991.8582445194642</v>
       </c>
       <c r="AK18" t="n">
-        <v>991.8582445194642</v>
+        <v>34.19612794612795</v>
       </c>
       <c r="AL18" t="n">
-        <v>34.19612794612795</v>
+        <v>6.839225589225591</v>
       </c>
       <c r="AM18" t="n">
-        <v>6.839225589225591</v>
+        <v>4.336947456213191</v>
       </c>
       <c r="AN18" t="n">
-        <v>4.336947456213191</v>
-      </c>
-      <c r="AO18" t="inlineStr"/>
-      <c r="AP18" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -3081,75 +2996,72 @@
       <c r="R19" t="n">
         <v>10.30922431865884</v>
       </c>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="n">
+        <v>11.85266229029905</v>
+      </c>
       <c r="T19" t="n">
+        <v>0.04225548053582551</v>
+      </c>
+      <c r="U19" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="U19" t="n">
-        <v>0.04225548053582551</v>
-      </c>
       <c r="V19" t="n">
+        <v>0.0794999999999942</v>
+      </c>
+      <c r="W19" t="n">
+        <v>51.99999999999621</v>
+      </c>
+      <c r="X19" t="n">
+        <v>4.336947456213196</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>41.33999999999698</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>52.00000000000001</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>8888.888888888891</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>39.00000000000002</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>54.16666666666669</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.09999999999999987</v>
+      </c>
+      <c r="AF19" t="n">
         <v>11.85266229029905</v>
       </c>
-      <c r="W19" t="n">
-        <v>0.0794999999999942</v>
-      </c>
-      <c r="X19" t="n">
-        <v>51.99999999999621</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>4.336947456213196</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>41.33999999999698</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>52.00000000000001</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>8888.888888888891</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>39.00000000000002</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>54.16666666666669</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>0.09999999999999987</v>
-      </c>
       <c r="AG19" t="n">
-        <v>11.85266229029905</v>
+        <v>52</v>
       </c>
       <c r="AH19" t="n">
-        <v>52</v>
+        <v>12.03703703703704</v>
       </c>
       <c r="AI19" t="n">
-        <v>12.03703703703704</v>
+        <v>21.888</v>
       </c>
       <c r="AJ19" t="n">
-        <v>21.888</v>
+        <v>969.6662445194643</v>
       </c>
       <c r="AK19" t="n">
-        <v>969.6662445194643</v>
+        <v>34.19612794612796</v>
       </c>
       <c r="AL19" t="n">
-        <v>34.19612794612796</v>
+        <v>6.839225589225592</v>
       </c>
       <c r="AM19" t="n">
-        <v>6.839225589225592</v>
+        <v>4.336947456213195</v>
       </c>
       <c r="AN19" t="n">
-        <v>4.336947456213195</v>
-      </c>
-      <c r="AO19" t="inlineStr"/>
-      <c r="AP19" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -3208,75 +3120,72 @@
       <c r="R20" t="n">
         <v>0</v>
       </c>
-      <c r="S20" t="inlineStr"/>
+      <c r="S20" t="n">
+        <v>10.78976462115079</v>
+      </c>
       <c r="T20" t="n">
+        <v>0.03846618403262313</v>
+      </c>
+      <c r="U20" t="n">
         <v>10.78976462115079</v>
       </c>
-      <c r="U20" t="n">
-        <v>0.03846618403262313</v>
-      </c>
       <c r="V20" t="n">
+        <v>0.07237076923077039</v>
+      </c>
+      <c r="W20" t="n">
+        <v>47.33685534591272</v>
+      </c>
+      <c r="X20" t="n">
+        <v>3.94802796880006</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>37.63280000000061</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>52</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>8888.888888888889</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>39.00000000000001</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>22.15909090909092</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>49.3092243186591</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.09999999999999987</v>
+      </c>
+      <c r="AF20" t="n">
         <v>10.78976462115079</v>
       </c>
-      <c r="W20" t="n">
-        <v>0.07237076923077039</v>
-      </c>
-      <c r="X20" t="n">
+      <c r="AG20" t="n">
         <v>47.33685534591272</v>
       </c>
-      <c r="Y20" t="n">
-        <v>3.94802796880006</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>37.63280000000061</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>52</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>39.00000000000001</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>22.15909090909092</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>49.3092243186591</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0.09999999999999987</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>10.78976462115079</v>
-      </c>
       <c r="AH20" t="n">
-        <v>47.33685534591272</v>
+        <v>10.95760540414646</v>
       </c>
       <c r="AI20" t="n">
-        <v>10.95760540414646</v>
+        <v>3.344</v>
       </c>
       <c r="AJ20" t="n">
-        <v>3.344</v>
+        <v>951.1331630467366</v>
       </c>
       <c r="AK20" t="n">
-        <v>951.1331630467366</v>
+        <v>33.11669631323738</v>
       </c>
       <c r="AL20" t="n">
-        <v>33.11669631323738</v>
+        <v>6.623339262647476</v>
       </c>
       <c r="AM20" t="n">
-        <v>6.623339262647476</v>
+        <v>3.948027968800059</v>
       </c>
       <c r="AN20" t="n">
-        <v>3.948027968800059</v>
-      </c>
-      <c r="AO20" t="inlineStr"/>
-      <c r="AP20" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -3335,75 +3244,72 @@
       <c r="R21" t="n">
         <v>0</v>
       </c>
-      <c r="S21" t="inlineStr"/>
+      <c r="S21" t="n">
+        <v>4.863433476000979</v>
+      </c>
       <c r="T21" t="n">
+        <v>0.01733844376470937</v>
+      </c>
+      <c r="U21" t="n">
         <v>4.863433476000979</v>
       </c>
-      <c r="U21" t="n">
-        <v>0.01733844376470937</v>
-      </c>
       <c r="V21" t="n">
+        <v>0.03262076923076852</v>
+      </c>
+      <c r="W21" t="n">
+        <v>21.33685534591149</v>
+      </c>
+      <c r="X21" t="n">
+        <v>1.779554240693202</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>16.96279999999963</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>29.6345213137668</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>5065.730139105436</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>22.22589098532511</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>12.6283471507529</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>22.22589098532447</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.09999999999999987</v>
+      </c>
+      <c r="AF21" t="n">
         <v>4.863433476000979</v>
       </c>
-      <c r="W21" t="n">
-        <v>0.03262076923076852</v>
-      </c>
-      <c r="X21" t="n">
+      <c r="AG21" t="n">
         <v>21.33685534591149</v>
       </c>
-      <c r="Y21" t="n">
-        <v>1.779554240693202</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>16.96279999999963</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>29.6345213137668</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>5065.730139105436</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>22.22589098532511</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>12.6283471507529</v>
-      </c>
-      <c r="AE21" t="n">
-        <v>22.22589098532447</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0.09999999999999987</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>4.863433476000979</v>
-      </c>
       <c r="AH21" t="n">
-        <v>21.33685534591149</v>
+        <v>4.939086885627659</v>
       </c>
       <c r="AI21" t="n">
-        <v>4.939086885627659</v>
+        <v>0</v>
       </c>
       <c r="AJ21" t="n">
         <v>0</v>
       </c>
       <c r="AK21" t="n">
-        <v>0</v>
+        <v>17.56743403638056</v>
       </c>
       <c r="AL21" t="n">
-        <v>17.56743403638056</v>
+        <v>3.513486807276113</v>
       </c>
       <c r="AM21" t="n">
-        <v>3.513486807276113</v>
+        <v>1.779554240693201</v>
       </c>
       <c r="AN21" t="n">
-        <v>1.779554240693201</v>
-      </c>
-      <c r="AO21" t="inlineStr"/>
-      <c r="AP21" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -3462,75 +3368,72 @@
       <c r="R22" t="n">
         <v>0</v>
       </c>
-      <c r="S22" t="inlineStr"/>
+      <c r="S22" t="n">
+        <v>-3.189146243560057e-14</v>
+      </c>
       <c r="T22" t="n">
+        <v>-1.136950532463478e-16</v>
+      </c>
+      <c r="U22" t="n">
         <v>-3.189146243560057e-14</v>
       </c>
-      <c r="U22" t="n">
-        <v>-1.136950532463478e-16</v>
-      </c>
       <c r="V22" t="n">
+        <v>-2.139073232268963e-16</v>
+      </c>
+      <c r="W22" t="n">
+        <v>-1.399142239974668e-13</v>
+      </c>
+      <c r="X22" t="n">
+        <v>-1.166924303565194e-14</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>-1.112318080779861e-13</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>-1.457439833306946e-13</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.09999999999999987</v>
+      </c>
+      <c r="AF22" t="n">
         <v>-3.189146243560057e-14</v>
       </c>
-      <c r="W22" t="n">
-        <v>-2.139073232268963e-16</v>
-      </c>
-      <c r="X22" t="n">
+      <c r="AG22" t="n">
         <v>-1.399142239974668e-13</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="AH22" t="n">
+        <v>-3.238755185126545e-14</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>-3.238755185126545e-14</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>-6.477510370253091e-15</v>
+      </c>
+      <c r="AM22" t="n">
         <v>-1.166924303565194e-14</v>
       </c>
-      <c r="Z22" t="n">
-        <v>-1.112318080779861e-13</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>-1.457439833306946e-13</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>0.09999999999999987</v>
-      </c>
-      <c r="AG22" t="n">
-        <v>-3.189146243560057e-14</v>
-      </c>
-      <c r="AH22" t="n">
-        <v>-1.399142239974668e-13</v>
-      </c>
-      <c r="AI22" t="n">
-        <v>-3.238755185126545e-14</v>
-      </c>
-      <c r="AJ22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL22" t="n">
-        <v>-3.238755185126545e-14</v>
-      </c>
-      <c r="AM22" t="n">
-        <v>-6.477510370253091e-15</v>
-      </c>
       <c r="AN22" t="n">
-        <v>-1.166924303565194e-14</v>
-      </c>
-      <c r="AO22" t="inlineStr"/>
-      <c r="AP22" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -3589,7 +3492,9 @@
       <c r="R23" t="n">
         <v>0</v>
       </c>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
       <c r="T23" t="n">
         <v>0</v>
       </c>
@@ -3651,13 +3556,8 @@
         <v>0</v>
       </c>
       <c r="AN23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO23" t="inlineStr"/>
-      <c r="AP23" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -3716,7 +3616,9 @@
       <c r="R24" t="n">
         <v>0</v>
       </c>
-      <c r="S24" t="inlineStr"/>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
       <c r="T24" t="n">
         <v>0</v>
       </c>
@@ -3766,10 +3668,10 @@
         <v>0</v>
       </c>
       <c r="AJ24" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AK24" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL24" t="n">
         <v>0</v>
@@ -3778,13 +3680,8 @@
         <v>0</v>
       </c>
       <c r="AN24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO24" t="inlineStr"/>
-      <c r="AP24" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -3843,75 +3740,72 @@
       <c r="R25" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="n">
+        <v>-1.238503395557304e-15</v>
+      </c>
       <c r="T25" t="n">
+        <v>-4.415341873644577e-18</v>
+      </c>
+      <c r="U25" t="n">
         <v>-1.238503395557304e-15</v>
       </c>
-      <c r="U25" t="n">
-        <v>-4.415341873644577e-18</v>
-      </c>
       <c r="V25" t="n">
-        <v>-1.238503395557304e-15</v>
+        <v>-8.307080513665876e-18</v>
       </c>
       <c r="W25" t="n">
-        <v>-8.307080513665876e-18</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="X25" t="n">
+        <v>-4.531744868214346e-16</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>-4.319681867106255e-15</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>-7.546614023595834e-15</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>-1.290019491212963e-12</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>-5.659960517696877e-15</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>-3.215886657782316e-15</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>-5.659960517696878e-15</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>-1.0449157878825e-17</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>-1.238503395557303e-15</v>
+      </c>
+      <c r="AG25" t="n">
         <v>-5.433562096989001e-15</v>
       </c>
-      <c r="Y25" t="n">
+      <c r="AH25" t="n">
+        <v>-1.257769003932639e-15</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>-4.473655661714955e-15</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>-8.947311323429911e-16</v>
+      </c>
+      <c r="AM25" t="n">
         <v>-4.531744868214346e-16</v>
       </c>
-      <c r="Z25" t="n">
-        <v>-4.319681867106255e-15</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>-7.546614023595834e-15</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>-1.290019491212963e-12</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>-5.659960517696877e-15</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>-3.215886657782316e-15</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>-5.659960517696878e-15</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>-1.0449157878825e-17</v>
-      </c>
-      <c r="AG25" t="n">
-        <v>-1.238503395557303e-15</v>
-      </c>
-      <c r="AH25" t="n">
-        <v>-5.433562096989001e-15</v>
-      </c>
-      <c r="AI25" t="n">
-        <v>-1.257769003932639e-15</v>
-      </c>
-      <c r="AJ25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK25" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AL25" t="n">
-        <v>-4.473655661714955e-15</v>
-      </c>
-      <c r="AM25" t="n">
-        <v>-8.947311323429911e-16</v>
-      </c>
       <c r="AN25" t="n">
-        <v>-4.531744868214346e-16</v>
-      </c>
-      <c r="AO25" t="inlineStr"/>
-      <c r="AP25" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -3970,75 +3864,72 @@
       <c r="R26" t="n">
         <v>0</v>
       </c>
-      <c r="S26" t="inlineStr"/>
+      <c r="S26" t="n">
+        <v>-1.238503395557304e-15</v>
+      </c>
       <c r="T26" t="n">
+        <v>-4.415341873644577e-18</v>
+      </c>
+      <c r="U26" t="n">
         <v>-1.238503395557304e-15</v>
       </c>
-      <c r="U26" t="n">
-        <v>-4.415341873644577e-18</v>
-      </c>
       <c r="V26" t="n">
-        <v>-1.238503395557304e-15</v>
+        <v>-8.307080513665876e-18</v>
       </c>
       <c r="W26" t="n">
-        <v>-8.307080513665876e-18</v>
+        <v>-5.433562096989001e-15</v>
       </c>
       <c r="X26" t="n">
+        <v>-4.531744868214346e-16</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>-4.319681867106255e-15</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>-7.546614023595834e-15</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>-1.290019491212963e-12</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>-5.659960517696877e-15</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>-3.215886657782316e-15</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>-5.659960517696878e-15</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>-1.0449157878825e-17</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>-1.238503395557303e-15</v>
+      </c>
+      <c r="AG26" t="n">
         <v>-5.433562096989001e-15</v>
       </c>
-      <c r="Y26" t="n">
+      <c r="AH26" t="n">
+        <v>-1.257769003932639e-15</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>-4.473655661714955e-15</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>-8.947311323429911e-16</v>
+      </c>
+      <c r="AM26" t="n">
         <v>-4.531744868214346e-16</v>
       </c>
-      <c r="Z26" t="n">
-        <v>-4.319681867106255e-15</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>-7.546614023595834e-15</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>-1.290019491212963e-12</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>-5.659960517696877e-15</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>-3.215886657782316e-15</v>
-      </c>
-      <c r="AE26" t="n">
-        <v>-5.659960517696878e-15</v>
-      </c>
-      <c r="AF26" t="n">
-        <v>-1.0449157878825e-17</v>
-      </c>
-      <c r="AG26" t="n">
-        <v>-1.238503395557303e-15</v>
-      </c>
-      <c r="AH26" t="n">
-        <v>-5.433562096989001e-15</v>
-      </c>
-      <c r="AI26" t="n">
-        <v>-1.257769003932639e-15</v>
-      </c>
-      <c r="AJ26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AL26" t="n">
-        <v>-4.473655661714955e-15</v>
-      </c>
-      <c r="AM26" t="n">
-        <v>-8.947311323429911e-16</v>
-      </c>
       <c r="AN26" t="n">
-        <v>-4.531744868214346e-16</v>
-      </c>
-      <c r="AO26" t="inlineStr"/>
-      <c r="AP26" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -4097,75 +3988,124 @@
       <c r="R27" t="n">
         <v>0</v>
       </c>
-      <c r="S27" t="inlineStr"/>
+      <c r="S27" t="n">
+        <v>-4.358010037207033e-14</v>
+      </c>
       <c r="T27" t="n">
+        <v>-1.553657767275235e-16</v>
+      </c>
+      <c r="U27" t="n">
         <v>-4.358010037207033e-14</v>
       </c>
-      <c r="U27" t="n">
-        <v>-1.553657767275235e-16</v>
-      </c>
       <c r="V27" t="n">
+        <v>-2.923071538463765e-16</v>
+      </c>
+      <c r="W27" t="n">
+        <v>-1.911946163523469e-13</v>
+      </c>
+      <c r="X27" t="n">
+        <v>-1.594617317367364e-14</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>-1.519997200001158e-13</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>-2.655480782671485e-13</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>-4.539283389182025e-11</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>-1.991610587003614e-13</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>-1.131596924433872e-13</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>-1.991610587003614e-13</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>-1.0449157878825e-17</v>
+      </c>
+      <c r="AF27" t="n">
         <v>-4.358010037207033e-14</v>
       </c>
-      <c r="W27" t="n">
-        <v>-2.923071538463765e-16</v>
-      </c>
-      <c r="X27" t="n">
+      <c r="AG27" t="n">
         <v>-1.911946163523469e-13</v>
       </c>
-      <c r="Y27" t="n">
-        <v>-1.594617317367364e-14</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>-1.519997200001158e-13</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>-2.655480782671485e-13</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>-4.539283389182025e-11</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>-1.991610587003614e-13</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>-1.131596924433872e-13</v>
-      </c>
-      <c r="AE27" t="n">
-        <v>-1.991610587003614e-13</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>-1.0449157878825e-17</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>-4.358010037207033e-14</v>
-      </c>
       <c r="AH27" t="n">
-        <v>-1.911946163523469e-13</v>
+        <v>-4.425801304452475e-14</v>
       </c>
       <c r="AI27" t="n">
-        <v>-4.425801304452475e-14</v>
+        <v>0</v>
       </c>
       <c r="AJ27" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AK27" t="n">
-        <v>1000</v>
+        <v>-1.574177054879119e-13</v>
       </c>
       <c r="AL27" t="n">
-        <v>-1.574177054879119e-13</v>
+        <v>-3.148354109758239e-14</v>
       </c>
       <c r="AM27" t="n">
-        <v>-3.148354109758239e-14</v>
+        <v>-1.594617317367363e-14</v>
       </c>
       <c r="AN27" t="n">
-        <v>-1.594617317367363e-14</v>
-      </c>
-      <c r="AO27" t="inlineStr"/>
-      <c r="AP27" t="n">
         <v>-0</v>
       </c>
-      <c r="AQ27" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total_cost</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PV_revenue</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total_adjusted_cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_costs_toy__</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-94427.62279218005</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-94427.62279218005</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>